<commit_message>
Changed name of gen_trip and found a base for the 2030 scenario
</commit_message>
<xml_diff>
--- a/inertia_sim/2030_scenario/dataframes_transparency.xlsx
+++ b/inertia_sim/2030_scenario/dataframes_transparency.xlsx
@@ -522,7 +522,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="2">
-        <v>6403</v>
+        <v>6066</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
@@ -530,7 +530,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="2">
-        <v>1166</v>
+        <v>1104</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
@@ -538,7 +538,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="2">
-        <v>3978</v>
+        <v>3768</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
@@ -546,7 +546,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="2">
-        <v>1879</v>
+        <v>1781</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
@@ -554,7 +554,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="2">
-        <v>3352</v>
+        <v>3175</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
@@ -562,7 +562,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="2">
-        <v>2047</v>
+        <v>1939</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
@@ -570,7 +570,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="2">
-        <v>2605</v>
+        <v>2468</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
@@ -578,7 +578,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="2">
-        <v>5178</v>
+        <v>4905</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
@@ -586,7 +586,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="2">
-        <v>7684</v>
+        <v>7280</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
@@ -594,7 +594,7 @@
         <v>25</v>
       </c>
       <c r="B11" s="2">
-        <v>1729</v>
+        <v>1638</v>
       </c>
     </row>
   </sheetData>
@@ -762,7 +762,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>-1400</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
@@ -770,7 +770,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3">
-        <v>-1400</v>
+        <v>-700</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
@@ -810,7 +810,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="3">
-        <v>700</v>
+        <v>-700</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">

</xml_diff>

<commit_message>
Finished a base case for the 2030 scenario
</commit_message>
<xml_diff>
--- a/inertia_sim/2030_scenario/dataframes_transparency.xlsx
+++ b/inertia_sim/2030_scenario/dataframes_transparency.xlsx
@@ -505,7 +505,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="5" width="18.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
@@ -613,8 +613,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -722,7 +722,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="4" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">

</xml_diff>